<commit_message>
Preparation for transport: - Independent num/denum conversion - Added some passenger convs - CAP2ACT is now entity dependent
</commit_message>
<xml_diff>
--- a/data/raw_files/Ref_list.xlsx
+++ b/data/raw_files/Ref_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/raw_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98880990-1644-3C43-960C-FB83CD553E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0AB133-E96B-9146-8631-B50EB398DC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="1180" windowWidth="21600" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Author</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>https://www.swissgrid.ch/de/home/customers/topics/energy-data-ch.html</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Transport fuel prices and taxes in Europe</t>
+  </si>
+  <si>
+    <t>European Environment Agency</t>
+  </si>
+  <si>
+    <t>1980-2018</t>
+  </si>
+  <si>
+    <t>gasoline, diesel</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>Nominal cost of fuel</t>
+  </si>
+  <si>
+    <t>https://www.eea.europa.eu/data-and-maps/indicators/fuel-prices-and-taxes/assessment-4</t>
   </si>
 </sst>
 </file>
@@ -572,9 +596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,8 +756,34 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I6" s="3"/>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I7" s="3"/>
@@ -2272,6 +2322,7 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" location="kw-86936" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{F2BFD8CD-E70A-114E-AF72-6791AD923A9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>